<commit_message>
Update 1017 7 PM
</commit_message>
<xml_diff>
--- a/Data/GGEE_23_Camps.xlsx
+++ b/Data/GGEE_23_Camps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristadulany/Documents/GitHub/GGEESummer23/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristachisholm/Documents/GitHub/GGEESummer23/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BC9E1D-2DC8-A744-86E0-FDE3D849F6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464C3B61-09D4-B143-9616-D890533E9559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="500" windowWidth="43640" windowHeight="24700" xr2:uid="{1283F353-05F4-2D4F-9034-1D459AACA143}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16920" xr2:uid="{1283F353-05F4-2D4F-9034-1D459AACA143}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -917,7 +917,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:D23"/>
+      <selection activeCell="F11" sqref="F11:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>